<commit_message>
added SalivaMeanSeDataFrame as new type; renamed other functions
</commit_message>
<xml_diff>
--- a/example_data/saliva_sample_mean_se.xlsx
+++ b/example_data/saliva_sample_mean_se.xlsx
@@ -1,33 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10502"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Richer/Documents/PhD/Projects/BioPsyKit/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEC0EDC-8BF8-CF4D-A850-2D061CB3B070}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A313F693-51C7-EC47-AFC2-00487C6103B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" activeTab="1" xr2:uid="{5BEFDD1D-5847-0149-9B01-2968EF563D33}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" activeTab="2" xr2:uid="{5BEFDD1D-5847-0149-9B01-2968EF563D33}"/>
   </bookViews>
   <sheets>
     <sheet name="cortisol" sheetId="2" r:id="rId1"/>
     <sheet name="amylase" sheetId="3" r:id="rId2"/>
     <sheet name="il6" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>mean</t>
   </si>
@@ -37,12 +46,15 @@
   <si>
     <t>time</t>
   </si>
+  <si>
+    <t>sample</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -53,6 +65,17 @@
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,13 +98,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,106 +428,125 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
       <c r="B2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C2" s="1">
         <v>8.0039999999999996</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>1.0209999999999999</v>
       </c>
-      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10.750999999999999</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>14.33</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
         <v>20</v>
       </c>
-      <c r="B3" s="1">
-        <v>10.750999999999999</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.83199999999999996</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>30</v>
-      </c>
-      <c r="B4" s="1">
-        <v>14.33</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1.23</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>40</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>13.641</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>1.3380000000000001</v>
       </c>
-      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>65</v>
+      <c r="A6" s="4">
+        <v>4</v>
       </c>
       <c r="B6" s="1">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1">
         <v>10.548999999999999</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>1.036</v>
       </c>
-      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>80</v>
+      <c r="A7" s="4">
+        <v>5</v>
       </c>
       <c r="B7" s="1">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1">
         <v>8.0850000000000009</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>0.67200000000000004</v>
       </c>
-      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>140</v>
+      <c r="A8" s="4">
+        <v>6</v>
       </c>
       <c r="B8" s="1">
+        <v>120</v>
+      </c>
+      <c r="C8" s="1">
         <v>6.6260000000000003</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>0.47899999999999998</v>
       </c>
-      <c r="D8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -509,106 +557,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFC73B9-8B52-FC4A-9704-CA65E59813C0}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
       <c r="B2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C2" s="1">
         <v>106.381</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>16.885000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>212.55</v>
+      </c>
+      <c r="D3" s="1">
+        <v>26.635000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>169.303</v>
+      </c>
+      <c r="D4" s="1">
+        <v>24.481000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
         <v>20</v>
       </c>
-      <c r="B3" s="1">
-        <v>212.55</v>
-      </c>
-      <c r="C3" s="1">
-        <v>26.635000000000002</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>30</v>
-      </c>
-      <c r="B4" s="1">
-        <v>169.303</v>
-      </c>
-      <c r="C4" s="1">
-        <v>24.481000000000002</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>40</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>141.1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>23.614999999999998</v>
       </c>
-      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>65</v>
+      <c r="A6" s="4">
+        <v>4</v>
       </c>
       <c r="B6" s="1">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1">
         <v>161.34299999999999</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>26.427</v>
       </c>
-      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>80</v>
+      <c r="A7" s="4">
+        <v>5</v>
       </c>
       <c r="B7" s="1">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1">
         <v>142.80600000000001</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>22.271000000000001</v>
       </c>
-      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>140</v>
+      <c r="A8" s="4">
+        <v>6</v>
       </c>
       <c r="B8" s="1">
+        <v>120</v>
+      </c>
+      <c r="C8" s="1">
         <v>140.917</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>22.423999999999999</v>
       </c>
-      <c r="D8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -619,52 +687,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8473BD-A2FF-A541-BED6-0085648ED183}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="10.83203125" style="4"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C2" s="7">
         <v>0.70199999999999996</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="7">
         <v>0.112</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>50</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>30</v>
+      </c>
+      <c r="C3" s="7">
         <v>1.3740000000000001</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="7">
         <v>0.23699999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>140</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7">
+        <v>120</v>
+      </c>
+      <c r="C4" s="7">
         <v>4.0110000000000001</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="7">
         <v>0.72199999999999998</v>
       </c>
     </row>

</xml_diff>